<commit_message>
perfect on small loads, overestimates by 1 GPa on large loads
</commit_message>
<xml_diff>
--- a/data/data_error_analysis.xlsx
+++ b/data/data_error_analysis.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
   <si>
     <t>Load</t>
   </si>
@@ -281,6 +281,15 @@
   <si>
     <t>Redone AFM #2</t>
   </si>
+  <si>
+    <t>0.4 threshold</t>
+  </si>
+  <si>
+    <t>0.55 threshold</t>
+  </si>
+  <si>
+    <t>Metallization #2</t>
+  </si>
 </sst>
 </file>
 
@@ -417,8 +426,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="367">
+  <cellStyleXfs count="381">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -848,7 +871,7 @@
     <xf numFmtId="2" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="367">
+  <cellStyles count="381">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1032,6 +1055,13 @@
     <cellStyle name="Followed Hyperlink" xfId="362" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="364" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="366" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="368" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="370" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="372" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="374" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1215,6 +1245,13 @@
     <cellStyle name="Hyperlink" xfId="361" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="363" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="365" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="367" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="369" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="371" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="373" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1744,11 +1781,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2095187304"/>
-        <c:axId val="2095508328"/>
+        <c:axId val="2141637000"/>
+        <c:axId val="2141642568"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2095187304"/>
+        <c:axId val="2141637000"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="-0.001"/>
@@ -1778,12 +1815,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095508328"/>
+        <c:crossAx val="2141642568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2095508328"/>
+        <c:axId val="2141642568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1812,7 +1849,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2095187304"/>
+        <c:crossAx val="2141637000"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2337,11 +2374,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073522232"/>
-        <c:axId val="2073527976"/>
+        <c:axId val="2139651352"/>
+        <c:axId val="2139657064"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073522232"/>
+        <c:axId val="2139651352"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
           <c:max val="-0.001"/>
@@ -2371,12 +2408,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073527976"/>
+        <c:crossAx val="2139657064"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2073527976"/>
+        <c:axId val="2139657064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2404,7 +2441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073522232"/>
+        <c:crossAx val="2139651352"/>
         <c:crosses val="max"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2875,11 +2912,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073564568"/>
-        <c:axId val="2073570120"/>
+        <c:axId val="2141657544"/>
+        <c:axId val="2141668056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073564568"/>
+        <c:axId val="2141657544"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -2907,12 +2944,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073570120"/>
+        <c:crossAx val="2141668056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2073570120"/>
+        <c:axId val="2141668056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0.0"/>
@@ -2949,7 +2986,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="high"/>
-        <c:crossAx val="2073564568"/>
+        <c:crossAx val="2141657544"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3028,7 +3065,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'LP, AFM'!$V$12:$V$14</c:f>
+                <c:f>'LP, AFM'!$W$12:$W$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -3046,7 +3083,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'LP, AFM'!$V$12:$V$14</c:f>
+                <c:f>'LP, AFM'!$W$12:$W$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -3065,7 +3102,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$T$12:$T$14</c:f>
+              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3083,7 +3120,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
+              <c:f>'LP, AFM'!$V$12:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3119,7 +3156,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'LP, AFM'!$X$12:$X$14</c:f>
+                <c:f>'LP, AFM'!$Y$12:$Y$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -3137,7 +3174,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'LP, AFM'!$X$12:$X$14</c:f>
+                <c:f>'LP, AFM'!$Y$12:$Y$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -3156,7 +3193,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$T$12:$T$14</c:f>
+              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3174,7 +3211,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$W$12:$W$14</c:f>
+              <c:f>'LP, AFM'!$X$12:$X$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3210,7 +3247,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'LP, AFM'!$Z$12:$Z$14</c:f>
+                <c:f>'LP, AFM'!$AA$12:$AA$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -3228,7 +3265,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'LP, AFM'!$Z$12:$Z$14</c:f>
+                <c:f>'LP, AFM'!$AA$12:$AA$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -3247,7 +3284,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$T$12:$T$14</c:f>
+              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3265,7 +3302,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$Y$12:$Y$14</c:f>
+              <c:f>'LP, AFM'!$Z$12:$Z$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -3291,11 +3328,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097077992"/>
-        <c:axId val="2097084248"/>
+        <c:axId val="2141739272"/>
+        <c:axId val="2141744760"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097077992"/>
+        <c:axId val="2141739272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3324,12 +3361,12 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097084248"/>
+        <c:crossAx val="2141744760"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2097084248"/>
+        <c:axId val="2141744760"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.5"/>
@@ -3360,7 +3397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097077992"/>
+        <c:crossAx val="2141739272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3738,11 +3775,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2097133912"/>
-        <c:axId val="2073601208"/>
+        <c:axId val="2141758264"/>
+        <c:axId val="2141763960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2097133912"/>
+        <c:axId val="2141758264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="3000.0"/>
@@ -3765,19 +3802,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073601208"/>
+        <c:crossAx val="2141763960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2073601208"/>
+        <c:axId val="2141763960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="550.0"/>
@@ -3814,7 +3850,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2097133912"/>
+        <c:crossAx val="2141758264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4082,7 +4118,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'LP, AFM'!$V$12:$V$14</c:f>
+                <c:f>'LP, AFM'!$W$12:$W$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -4100,7 +4136,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'LP, AFM'!$V$12:$V$14</c:f>
+                <c:f>'LP, AFM'!$W$12:$W$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -4119,7 +4155,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$T$12:$T$14</c:f>
+              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4137,7 +4173,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
+              <c:f>'LP, AFM'!$V$12:$V$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4173,7 +4209,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'LP, AFM'!$X$12:$X$14</c:f>
+                <c:f>'LP, AFM'!$Y$12:$Y$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -4191,7 +4227,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'LP, AFM'!$X$12:$X$14</c:f>
+                <c:f>'LP, AFM'!$Y$12:$Y$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -4210,7 +4246,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$T$12:$T$14</c:f>
+              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4228,7 +4264,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$W$12:$W$14</c:f>
+              <c:f>'LP, AFM'!$X$12:$X$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4264,7 +4300,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'LP, AFM'!$Z$12:$Z$14</c:f>
+                <c:f>'LP, AFM'!$AA$12:$AA$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -4282,7 +4318,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'LP, AFM'!$Z$12:$Z$14</c:f>
+                <c:f>'LP, AFM'!$AA$12:$AA$14</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
@@ -4301,7 +4337,7 @@
           </c:errBars>
           <c:xVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$T$12:$T$14</c:f>
+              <c:f>'LP, AFM'!$U$12:$U$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4319,7 +4355,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'LP, AFM'!$Y$12:$Y$14</c:f>
+              <c:f>'LP, AFM'!$Z$12:$Z$14</c:f>
               <c:numCache>
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
@@ -4345,11 +4381,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2073630616"/>
-        <c:axId val="2086817560"/>
+        <c:axId val="2139934552"/>
+        <c:axId val="2139939960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2073630616"/>
+        <c:axId val="2139934552"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4371,19 +4407,18 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2086817560"/>
+        <c:crossAx val="2139939960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="2086817560"/>
+        <c:axId val="2139939960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="4.5"/>
@@ -4406,14 +4441,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="2073630616"/>
+        <c:crossAx val="2139934552"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -4555,13 +4589,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>26</xdr:col>
+      <xdr:col>27</xdr:col>
       <xdr:colOff>160866</xdr:colOff>
       <xdr:row>3</xdr:row>
       <xdr:rowOff>42332</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>34</xdr:col>
+      <xdr:col>35</xdr:col>
       <xdr:colOff>25400</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>16933</xdr:rowOff>
@@ -9832,10 +9866,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:AP21"/>
+  <dimension ref="A2:AQ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="Q6" sqref="Q6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -9850,10 +9884,19 @@
     <col min="13" max="13" width="16.33203125" customWidth="1"/>
     <col min="14" max="15" width="10.83203125" style="42"/>
     <col min="16" max="16" width="16.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="42" width="10.83203125" style="42"/>
+    <col min="17" max="17" width="16.6640625" customWidth="1"/>
+    <col min="18" max="43" width="10.83203125" style="42"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:42">
+    <row r="2" spans="1:43">
+      <c r="P2" t="s">
+        <v>85</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="3" spans="1:43">
       <c r="B3" s="2" t="s">
         <v>0</v>
       </c>
@@ -9895,17 +9938,20 @@
       <c r="P3" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="Q3" s="41" t="s">
+      <c r="Q3" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="R3" s="41" t="s">
         <v>19</v>
       </c>
-      <c r="R3" s="41"/>
-      <c r="T3" t="s">
+      <c r="S3" s="41"/>
+      <c r="U3" t="s">
         <v>62</v>
       </c>
-      <c r="U3"/>
       <c r="V3"/>
-    </row>
-    <row r="4" spans="1:42" s="23" customFormat="1">
+      <c r="W3"/>
+    </row>
+    <row r="4" spans="1:43" s="23" customFormat="1">
       <c r="A4" s="42">
         <v>0.1</v>
       </c>
@@ -9948,17 +9994,19 @@
       <c r="P4" s="23">
         <v>35.9251</v>
       </c>
-      <c r="Q4" s="42"/>
+      <c r="Q4" s="23">
+        <v>32.744900000000001</v>
+      </c>
       <c r="R4" s="42"/>
       <c r="S4" s="42"/>
-      <c r="T4">
+      <c r="T4" s="42"/>
+      <c r="U4">
         <v>1</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>0.18703</v>
       </c>
-      <c r="V4"/>
-      <c r="W4" s="42"/>
+      <c r="W4"/>
       <c r="X4" s="42"/>
       <c r="Y4" s="42"/>
       <c r="Z4" s="42"/>
@@ -9978,8 +10026,9 @@
       <c r="AN4" s="42"/>
       <c r="AO4" s="42"/>
       <c r="AP4" s="42"/>
-    </row>
-    <row r="5" spans="1:42" s="23" customFormat="1">
+      <c r="AQ4" s="42"/>
+    </row>
+    <row r="5" spans="1:43" s="23" customFormat="1">
       <c r="A5" s="42"/>
       <c r="B5" s="23">
         <v>245</v>
@@ -10017,17 +10066,19 @@
       <c r="P5" s="53">
         <v>34.667000000000002</v>
       </c>
-      <c r="Q5" s="42"/>
+      <c r="Q5" s="53">
+        <v>33.024500000000003</v>
+      </c>
       <c r="R5" s="42"/>
       <c r="S5" s="42"/>
-      <c r="T5">
+      <c r="T5" s="42"/>
+      <c r="U5">
         <v>2</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>0.18687999999999999</v>
       </c>
-      <c r="V5"/>
-      <c r="W5" s="42"/>
+      <c r="W5"/>
       <c r="X5" s="42"/>
       <c r="Y5" s="42"/>
       <c r="Z5" s="42"/>
@@ -10047,8 +10098,9 @@
       <c r="AN5" s="42"/>
       <c r="AO5" s="42"/>
       <c r="AP5" s="42"/>
-    </row>
-    <row r="6" spans="1:42" s="23" customFormat="1">
+      <c r="AQ5" s="42"/>
+    </row>
+    <row r="6" spans="1:43" s="23" customFormat="1">
       <c r="A6" s="42"/>
       <c r="B6" s="23">
         <v>245</v>
@@ -10086,17 +10138,16 @@
       <c r="P6" s="23">
         <v>34.352499999999999</v>
       </c>
-      <c r="Q6" s="42"/>
       <c r="R6" s="42"/>
       <c r="S6" s="42"/>
-      <c r="T6">
+      <c r="T6" s="42"/>
+      <c r="U6">
         <v>3</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>0.18692</v>
       </c>
-      <c r="V6"/>
-      <c r="W6" s="42"/>
+      <c r="W6"/>
       <c r="X6" s="42"/>
       <c r="Y6" s="42"/>
       <c r="Z6" s="42"/>
@@ -10116,8 +10167,9 @@
       <c r="AN6" s="42"/>
       <c r="AO6" s="42"/>
       <c r="AP6" s="42"/>
-    </row>
-    <row r="7" spans="1:42" s="23" customFormat="1">
+      <c r="AQ6" s="42"/>
+    </row>
+    <row r="7" spans="1:43" s="23" customFormat="1">
       <c r="A7" s="42"/>
       <c r="B7" s="23">
         <v>245</v>
@@ -10158,18 +10210,20 @@
       <c r="P7" s="23">
         <v>34.806800000000003</v>
       </c>
-      <c r="Q7" s="42"/>
+      <c r="Q7" s="23">
+        <v>32.465400000000002</v>
+      </c>
       <c r="R7" s="42"/>
       <c r="S7" s="42"/>
-      <c r="T7" t="s">
+      <c r="T7" s="42"/>
+      <c r="U7" t="s">
         <v>34</v>
       </c>
-      <c r="U7" s="55">
-        <f>AVERAGE(U4:U6)</f>
+      <c r="V7" s="55">
+        <f>AVERAGE(V4:V6)</f>
         <v>0.18694333333333332</v>
       </c>
-      <c r="V7" s="55"/>
-      <c r="W7" s="42"/>
+      <c r="W7" s="55"/>
       <c r="X7" s="42"/>
       <c r="Y7" s="42"/>
       <c r="Z7" s="42"/>
@@ -10189,8 +10243,9 @@
       <c r="AN7" s="42"/>
       <c r="AO7" s="42"/>
       <c r="AP7" s="42"/>
-    </row>
-    <row r="8" spans="1:42" s="23" customFormat="1">
+      <c r="AQ7" s="42"/>
+    </row>
+    <row r="8" spans="1:43" s="23" customFormat="1">
       <c r="A8" s="42"/>
       <c r="C8" s="25" t="s">
         <v>34</v>
@@ -10232,21 +10287,24 @@
         <f>AVERAGE(P4:P7)</f>
         <v>34.937850000000005</v>
       </c>
-      <c r="Q8" s="45">
+      <c r="Q8" s="26">
+        <f>AVERAGE(Q4:Q7)</f>
+        <v>32.744933333333336</v>
+      </c>
+      <c r="R8" s="45">
         <f>B4/P8</f>
         <v>7.0124521113920855</v>
       </c>
-      <c r="R8" s="45"/>
-      <c r="S8" s="42"/>
-      <c r="T8" t="s">
+      <c r="S8" s="45"/>
+      <c r="T8" s="42"/>
+      <c r="U8" t="s">
         <v>10</v>
       </c>
-      <c r="U8" s="55">
-        <f>STDEV(U4:U6)</f>
+      <c r="V8" s="55">
+        <f>STDEV(V4:V6)</f>
         <v>7.7674534651544719E-5</v>
       </c>
-      <c r="V8" s="55"/>
-      <c r="W8" s="42"/>
+      <c r="W8" s="55"/>
       <c r="X8" s="42"/>
       <c r="Y8" s="42"/>
       <c r="Z8" s="42"/>
@@ -10266,8 +10324,9 @@
       <c r="AN8" s="42"/>
       <c r="AO8" s="42"/>
       <c r="AP8" s="42"/>
-    </row>
-    <row r="9" spans="1:42" s="23" customFormat="1">
+      <c r="AQ8" s="42"/>
+    </row>
+    <row r="9" spans="1:43" s="23" customFormat="1">
       <c r="A9" s="42"/>
       <c r="C9" s="23" t="s">
         <v>10</v>
@@ -10315,15 +10374,18 @@
         <f>STDEV(P4:P7)</f>
         <v>0.68503795758580666</v>
       </c>
-      <c r="Q9" s="45">
-        <f>Q8*SQRT((0)^2+(P9/P8)^2)</f>
+      <c r="Q9" s="27">
+        <f>STDEV(Q4:Q7)</f>
+        <v>0.27955000149049108</v>
+      </c>
+      <c r="R9" s="45">
+        <f>R8*SQRT((0)^2+(P9/P8)^2)</f>
         <v>0.13749546328856271</v>
       </c>
-      <c r="R9" s="43">
-        <f>Q9/Q8*100</f>
+      <c r="S9" s="43">
+        <f>R9/R8*100</f>
         <v>1.9607330090025761</v>
       </c>
-      <c r="S9" s="42"/>
       <c r="T9" s="42"/>
       <c r="U9" s="42"/>
       <c r="V9" s="42"/>
@@ -10347,8 +10409,9 @@
       <c r="AN9" s="42"/>
       <c r="AO9" s="42"/>
       <c r="AP9" s="42"/>
-    </row>
-    <row r="10" spans="1:42" s="28" customFormat="1">
+      <c r="AQ9" s="42"/>
+    </row>
+    <row r="10" spans="1:43" s="28" customFormat="1">
       <c r="A10" s="42">
         <v>0.1</v>
       </c>
@@ -10391,7 +10454,6 @@
       <c r="P10" s="28">
         <v>67.726399999999998</v>
       </c>
-      <c r="Q10" s="42"/>
       <c r="R10" s="42"/>
       <c r="S10" s="42"/>
       <c r="T10" s="42"/>
@@ -10417,8 +10479,9 @@
       <c r="AN10" s="42"/>
       <c r="AO10" s="42"/>
       <c r="AP10" s="42"/>
-    </row>
-    <row r="11" spans="1:42" s="28" customFormat="1">
+      <c r="AQ10" s="42"/>
+    </row>
+    <row r="11" spans="1:43" s="28" customFormat="1">
       <c r="A11" s="42"/>
       <c r="B11" s="28">
         <v>490</v>
@@ -10439,31 +10502,30 @@
       <c r="P11" s="28">
         <v>77.476500000000001</v>
       </c>
-      <c r="Q11" s="42"/>
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
-      <c r="T11" s="42" t="s">
+      <c r="T11" s="42"/>
+      <c r="U11" s="42" t="s">
         <v>0</v>
       </c>
-      <c r="U11" s="42" t="s">
+      <c r="V11" s="42" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="42" t="s">
+      <c r="W11" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="W11" s="42" t="s">
+      <c r="X11" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="X11" s="42" t="s">
+      <c r="Y11" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="Y11" s="42" t="s">
+      <c r="Z11" s="42" t="s">
         <v>65</v>
       </c>
-      <c r="Z11" s="42" t="s">
+      <c r="AA11" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="AA11" s="42"/>
       <c r="AB11" s="42"/>
       <c r="AC11" s="42"/>
       <c r="AD11" s="42"/>
@@ -10479,8 +10541,9 @@
       <c r="AN11" s="42"/>
       <c r="AO11" s="42"/>
       <c r="AP11" s="42"/>
-    </row>
-    <row r="12" spans="1:42" s="28" customFormat="1">
+      <c r="AQ11" s="42"/>
+    </row>
+    <row r="12" spans="1:43" s="28" customFormat="1">
       <c r="A12" s="42"/>
       <c r="B12" s="28">
         <v>490</v>
@@ -10518,37 +10581,36 @@
       <c r="P12" s="28">
         <v>66.608199999999997</v>
       </c>
-      <c r="Q12" s="42"/>
       <c r="R12" s="42"/>
       <c r="S12" s="42"/>
-      <c r="T12" s="42">
+      <c r="T12" s="42"/>
+      <c r="U12" s="42">
         <v>245.2</v>
       </c>
-      <c r="U12" s="56">
+      <c r="V12" s="56">
         <f>N8</f>
         <v>7.4285025579063149</v>
       </c>
-      <c r="V12" s="56">
+      <c r="W12" s="56">
         <f>N9</f>
         <v>0.19061527768597833</v>
       </c>
-      <c r="W12" s="56">
+      <c r="X12" s="56">
         <f>F8</f>
         <v>6.2315068377010396</v>
       </c>
-      <c r="X12" s="56">
+      <c r="Y12" s="56">
         <f>F9</f>
         <v>0.51346301269000694</v>
       </c>
-      <c r="Y12" s="56">
-        <f>Q8</f>
+      <c r="Z12" s="56">
+        <f>R8</f>
         <v>7.0124521113920855</v>
       </c>
-      <c r="Z12" s="56">
-        <f>Q9</f>
+      <c r="AA12" s="56">
+        <f>R9</f>
         <v>0.13749546328856271</v>
       </c>
-      <c r="AA12" s="42"/>
       <c r="AB12" s="42"/>
       <c r="AC12" s="42"/>
       <c r="AD12" s="42"/>
@@ -10564,8 +10626,9 @@
       <c r="AN12" s="42"/>
       <c r="AO12" s="42"/>
       <c r="AP12" s="42"/>
-    </row>
-    <row r="13" spans="1:42" s="28" customFormat="1">
+      <c r="AQ12" s="42"/>
+    </row>
+    <row r="13" spans="1:43" s="28" customFormat="1">
       <c r="A13" s="42"/>
       <c r="B13" s="28">
         <v>490</v>
@@ -10603,37 +10666,36 @@
       <c r="P13" s="28">
         <v>71.116299999999995</v>
       </c>
-      <c r="Q13" s="42"/>
       <c r="R13" s="42"/>
       <c r="S13" s="42"/>
-      <c r="T13" s="42">
+      <c r="T13" s="42"/>
+      <c r="U13" s="42">
         <v>490.3</v>
       </c>
-      <c r="U13" s="56">
+      <c r="V13" s="56">
         <f>N14</f>
         <v>7.4087065910272996</v>
       </c>
-      <c r="V13" s="56">
+      <c r="W13" s="56">
         <f>N15</f>
         <v>9.9370122886482809E-2</v>
       </c>
-      <c r="W13" s="56">
+      <c r="X13" s="56">
         <f>F14</f>
         <v>6.4603173905591467</v>
       </c>
-      <c r="X13" s="56">
+      <c r="Y13" s="56">
         <f>F15</f>
         <v>0.40465434241416237</v>
       </c>
-      <c r="Y13" s="56">
-        <f>Q14</f>
+      <c r="Z13" s="56">
+        <f>R14</f>
         <v>6.9275722323111859</v>
       </c>
-      <c r="Z13" s="56">
-        <f>Q15</f>
+      <c r="AA13" s="56">
+        <f>R15</f>
         <v>0.47872956808486555</v>
       </c>
-      <c r="AA13" s="42"/>
       <c r="AB13" s="42"/>
       <c r="AC13" s="42"/>
       <c r="AD13" s="42"/>
@@ -10649,8 +10711,9 @@
       <c r="AN13" s="42"/>
       <c r="AO13" s="42"/>
       <c r="AP13" s="42"/>
-    </row>
-    <row r="14" spans="1:42" s="28" customFormat="1">
+      <c r="AQ13" s="42"/>
+    </row>
+    <row r="14" spans="1:43" s="28" customFormat="1">
       <c r="A14" s="42"/>
       <c r="C14" s="32" t="s">
         <v>34</v>
@@ -10692,40 +10755,43 @@
         <f>AVERAGE(P10:P13)</f>
         <v>70.731850000000009</v>
       </c>
-      <c r="Q14" s="43">
+      <c r="Q14" s="33" t="e">
+        <f>AVERAGE(Q10:Q13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R14" s="43">
         <f>B10/P14</f>
         <v>6.9275722323111859</v>
       </c>
-      <c r="R14" s="43"/>
-      <c r="S14" s="42"/>
-      <c r="T14" s="42">
+      <c r="S14" s="43"/>
+      <c r="T14" s="42"/>
+      <c r="U14" s="42">
         <v>2942</v>
       </c>
-      <c r="U14" s="56">
+      <c r="V14" s="56">
         <f>N20</f>
         <v>7.0826324979803248</v>
       </c>
-      <c r="V14" s="56">
+      <c r="W14" s="56">
         <f>N21</f>
         <v>0.32339382259507826</v>
       </c>
-      <c r="W14" s="56">
+      <c r="X14" s="56">
         <f>F20</f>
         <v>7.62883710799135</v>
       </c>
-      <c r="X14" s="56">
+      <c r="Y14" s="56">
         <f>F21</f>
         <v>0.1424828814607475</v>
       </c>
-      <c r="Y14" s="56">
-        <f>Q20</f>
+      <c r="Z14" s="56">
+        <f>R20</f>
         <v>7.92236264134766</v>
       </c>
-      <c r="Z14" s="56">
-        <f>Q21</f>
+      <c r="AA14" s="56">
+        <f>R21</f>
         <v>0.19460230294651493</v>
       </c>
-      <c r="AA14" s="42"/>
       <c r="AB14" s="42"/>
       <c r="AC14" s="42"/>
       <c r="AD14" s="42"/>
@@ -10741,8 +10807,9 @@
       <c r="AN14" s="42"/>
       <c r="AO14" s="42"/>
       <c r="AP14" s="42"/>
-    </row>
-    <row r="15" spans="1:42" s="28" customFormat="1">
+      <c r="AQ14" s="42"/>
+    </row>
+    <row r="15" spans="1:43" s="28" customFormat="1">
       <c r="A15" s="42"/>
       <c r="C15" s="28" t="s">
         <v>10</v>
@@ -10790,15 +10857,18 @@
         <f>STDEV(P10:P13)</f>
         <v>4.8879213185838708</v>
       </c>
-      <c r="Q15" s="43">
-        <f>Q14*SQRT((0)^2+(P15/P14)^2)</f>
+      <c r="Q15" s="34" t="e">
+        <f>STDEV(Q10:Q13)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R15" s="43">
+        <f>R14*SQRT((0)^2+(P15/P14)^2)</f>
         <v>0.47872956808486555</v>
       </c>
-      <c r="R15" s="43">
-        <f>Q15/Q14*100</f>
+      <c r="S15" s="43">
+        <f>R15/R14*100</f>
         <v>6.9104955102741839</v>
       </c>
-      <c r="S15" s="42"/>
       <c r="T15" s="42"/>
       <c r="U15" s="42"/>
       <c r="V15" s="42"/>
@@ -10822,8 +10892,9 @@
       <c r="AN15" s="42"/>
       <c r="AO15" s="42"/>
       <c r="AP15" s="42"/>
-    </row>
-    <row r="16" spans="1:42" s="7" customFormat="1">
+      <c r="AQ15" s="42"/>
+    </row>
+    <row r="16" spans="1:43" s="7" customFormat="1">
       <c r="A16" s="42">
         <v>1</v>
       </c>
@@ -10866,22 +10937,21 @@
       <c r="P16" s="7">
         <v>361.34750000000003</v>
       </c>
-      <c r="Q16" s="42"/>
       <c r="R16" s="42"/>
       <c r="S16" s="42"/>
       <c r="T16" s="42"/>
       <c r="U16" s="42"/>
       <c r="V16" s="42"/>
-      <c r="W16" s="42">
-        <f>(W12-U12)/U12*100</f>
+      <c r="W16" s="42"/>
+      <c r="X16" s="42">
+        <f>(X12-V12)/V12*100</f>
         <v>-16.113553315415999</v>
       </c>
-      <c r="X16" s="42"/>
-      <c r="Y16" s="42">
-        <f>(Y12-U12)/U12*100</f>
+      <c r="Y16" s="42"/>
+      <c r="Z16" s="42">
+        <f>(Z12-V12)/V12*100</f>
         <v>-5.6007310123548111</v>
       </c>
-      <c r="Z16" s="42"/>
       <c r="AA16" s="42"/>
       <c r="AB16" s="42"/>
       <c r="AC16" s="42"/>
@@ -10898,8 +10968,9 @@
       <c r="AN16" s="42"/>
       <c r="AO16" s="42"/>
       <c r="AP16" s="42"/>
-    </row>
-    <row r="17" spans="1:42" s="7" customFormat="1">
+      <c r="AQ16" s="42"/>
+    </row>
+    <row r="17" spans="1:43" s="7" customFormat="1">
       <c r="A17" s="42"/>
       <c r="B17" s="7">
         <v>2942</v>
@@ -10934,22 +11005,21 @@
       <c r="P17" s="7">
         <v>379.20519999999999</v>
       </c>
-      <c r="Q17" s="42"/>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
       <c r="U17" s="42"/>
       <c r="V17" s="42"/>
-      <c r="W17" s="42">
-        <f t="shared" ref="W17:W18" si="0">(W13-U13)/U13*100</f>
+      <c r="W17" s="42"/>
+      <c r="X17" s="42">
+        <f t="shared" ref="X17:X18" si="0">(X13-V13)/V13*100</f>
         <v>-12.801009040049568</v>
       </c>
-      <c r="X17" s="42"/>
-      <c r="Y17" s="42">
-        <f t="shared" ref="Y17:Y18" si="1">(Y13-U13)/U13*100</f>
+      <c r="Y17" s="42"/>
+      <c r="Z17" s="42">
+        <f t="shared" ref="Z17:Z18" si="1">(Z13-V13)/V13*100</f>
         <v>-6.4941748307162888</v>
       </c>
-      <c r="Z17" s="42"/>
       <c r="AA17" s="42"/>
       <c r="AB17" s="42"/>
       <c r="AC17" s="42"/>
@@ -10966,8 +11036,9 @@
       <c r="AN17" s="42"/>
       <c r="AO17" s="42"/>
       <c r="AP17" s="42"/>
-    </row>
-    <row r="18" spans="1:42" s="7" customFormat="1">
+      <c r="AQ17" s="42"/>
+    </row>
+    <row r="18" spans="1:43" s="7" customFormat="1">
       <c r="A18" s="42"/>
       <c r="B18" s="7">
         <v>2942</v>
@@ -11008,22 +11079,21 @@
       <c r="P18" s="7">
         <v>373.50889999999998</v>
       </c>
-      <c r="Q18" s="42"/>
       <c r="R18" s="42"/>
       <c r="S18" s="42"/>
       <c r="T18" s="42"/>
       <c r="U18" s="42"/>
       <c r="V18" s="42"/>
-      <c r="W18" s="42">
+      <c r="W18" s="42"/>
+      <c r="X18" s="42">
         <f t="shared" si="0"/>
         <v>7.7118869314026988</v>
       </c>
-      <c r="X18" s="42"/>
-      <c r="Y18" s="42">
+      <c r="Y18" s="42"/>
+      <c r="Z18" s="42">
         <f t="shared" si="1"/>
         <v>11.856186857171986</v>
       </c>
-      <c r="Z18" s="42"/>
       <c r="AA18" s="42"/>
       <c r="AB18" s="42"/>
       <c r="AC18" s="42"/>
@@ -11040,8 +11110,9 @@
       <c r="AN18" s="42"/>
       <c r="AO18" s="42"/>
       <c r="AP18" s="42"/>
-    </row>
-    <row r="19" spans="1:42" s="7" customFormat="1">
+      <c r="AQ18" s="42"/>
+    </row>
+    <row r="19" spans="1:43" s="7" customFormat="1">
       <c r="A19" s="42"/>
       <c r="B19" s="7">
         <v>2942</v>
@@ -11063,7 +11134,6 @@
       </c>
       <c r="N19" s="42"/>
       <c r="O19" s="42"/>
-      <c r="Q19" s="42"/>
       <c r="R19" s="42"/>
       <c r="S19" s="42"/>
       <c r="T19" s="42"/>
@@ -11089,8 +11159,9 @@
       <c r="AN19" s="42"/>
       <c r="AO19" s="42"/>
       <c r="AP19" s="42"/>
-    </row>
-    <row r="20" spans="1:42" s="7" customFormat="1">
+      <c r="AQ19" s="42"/>
+    </row>
+    <row r="20" spans="1:43" s="7" customFormat="1">
       <c r="A20" s="42"/>
       <c r="C20" s="39" t="s">
         <v>34</v>
@@ -11132,12 +11203,15 @@
         <f>AVERAGE(P16:P19)</f>
         <v>371.35386666666665</v>
       </c>
-      <c r="Q20" s="45">
+      <c r="Q20" s="40" t="e">
+        <f>AVERAGE(Q16:Q19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R20" s="45">
         <f>B16/P20</f>
         <v>7.92236264134766</v>
       </c>
-      <c r="R20" s="45"/>
-      <c r="S20" s="42"/>
+      <c r="S20" s="45"/>
       <c r="T20" s="42"/>
       <c r="U20" s="42"/>
       <c r="V20" s="42"/>
@@ -11161,8 +11235,9 @@
       <c r="AN20" s="42"/>
       <c r="AO20" s="42"/>
       <c r="AP20" s="42"/>
-    </row>
-    <row r="21" spans="1:42" s="7" customFormat="1">
+      <c r="AQ20" s="42"/>
+    </row>
+    <row r="21" spans="1:43" s="7" customFormat="1">
       <c r="A21" s="42"/>
       <c r="C21" s="7" t="s">
         <v>10</v>
@@ -11210,15 +11285,18 @@
         <f>STDEV(P16:P19)</f>
         <v>9.1218138998410279</v>
       </c>
-      <c r="Q21" s="45">
-        <f>Q20*SQRT((0)^2+(P21/P20)^2)</f>
+      <c r="Q21" s="19" t="e">
+        <f>STDEV(Q16:Q19)</f>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="R21" s="45">
+        <f>R20*SQRT((0)^2+(P21/P20)^2)</f>
         <v>0.19460230294651493</v>
       </c>
-      <c r="R21" s="43">
-        <f>Q21/Q20*100</f>
+      <c r="S21" s="43">
+        <f>R21/R20*100</f>
         <v>2.4563670177235339</v>
       </c>
-      <c r="S21" s="42"/>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
       <c r="V21" s="42"/>
@@ -11242,6 +11320,7 @@
       <c r="AN21" s="42"/>
       <c r="AO21" s="42"/>
       <c r="AP21" s="42"/>
+      <c r="AQ21" s="42"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
new matlab for indent corners
</commit_message>
<xml_diff>
--- a/data/data_error_analysis.xlsx
+++ b/data/data_error_analysis.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20910"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27240" windowHeight="14820" tabRatio="500" firstSheet="2" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="27240" windowHeight="14820" tabRatio="500" firstSheet="3" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Different Planes" sheetId="2" r:id="rId1"/>
@@ -14,6 +14,7 @@
     <sheet name="Before and After Gold 200nm" sheetId="7" r:id="rId5"/>
     <sheet name="LP, AFM" sheetId="8" r:id="rId6"/>
     <sheet name="Human Error" sheetId="9" r:id="rId7"/>
+    <sheet name="Diagonals" sheetId="10" r:id="rId8"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="98">
   <si>
     <t>Load</t>
   </si>
@@ -290,6 +291,36 @@
   <si>
     <t>Metallization #2</t>
   </si>
+  <si>
+    <t>Diagonal Area</t>
+  </si>
+  <si>
+    <t>Some variability</t>
+  </si>
+  <si>
+    <t>2942, #4</t>
+  </si>
+  <si>
+    <t>Try 1</t>
+  </si>
+  <si>
+    <t>Try 2</t>
+  </si>
+  <si>
+    <t>Try 3</t>
+  </si>
+  <si>
+    <t>Try 4</t>
+  </si>
+  <si>
+    <t>Stdev</t>
+  </si>
+  <si>
+    <t>AFM Square error</t>
+  </si>
+  <si>
+    <t>AFM Diagonals</t>
+  </si>
 </sst>
 </file>
 
@@ -426,8 +457,28 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="381">
+  <cellStyleXfs count="401">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -871,7 +922,7 @@
     <xf numFmtId="2" fontId="3" fillId="9" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="2" fontId="3" fillId="10" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="381">
+  <cellStyles count="401">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1062,6 +1113,16 @@
     <cellStyle name="Followed Hyperlink" xfId="376" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="378" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="380" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="382" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="384" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="386" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="388" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="390" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="392" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="394" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="396" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="398" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="400" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1252,6 +1313,16 @@
     <cellStyle name="Hyperlink" xfId="375" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="377" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="379" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="381" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="383" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="385" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="387" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="389" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="391" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="393" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="395" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="397" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="399" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -3252,13 +3323,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.137495463288563</c:v>
+                    <c:v>0.0638759485097753</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.478729568084866</c:v>
+                    <c:v>0.331837187948994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.194602302946515</c:v>
+                    <c:v>0.0307747817868176</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3270,13 +3341,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.137495463288563</c:v>
+                    <c:v>0.0638759485097753</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.478729568084866</c:v>
+                    <c:v>0.331837187948994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.194602302946515</c:v>
+                    <c:v>0.0307747817868176</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -3307,13 +3378,13 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.012452111392085</c:v>
+                  <c:v>7.482073562525703</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.927572232311186</c:v>
+                  <c:v>7.48506995867172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.92236264134766</c:v>
+                  <c:v>7.94804217325192</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3802,6 +3873,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4305,13 +4377,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.137495463288563</c:v>
+                    <c:v>0.0638759485097753</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.478729568084866</c:v>
+                    <c:v>0.331837187948994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.194602302946515</c:v>
+                    <c:v>0.0307747817868176</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -4323,13 +4395,13 @@
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="3"/>
                   <c:pt idx="0">
-                    <c:v>0.137495463288563</c:v>
+                    <c:v>0.0638759485097753</c:v>
                   </c:pt>
                   <c:pt idx="1">
-                    <c:v>0.478729568084866</c:v>
+                    <c:v>0.331837187948994</c:v>
                   </c:pt>
                   <c:pt idx="2">
-                    <c:v>0.194602302946515</c:v>
+                    <c:v>0.0307747817868176</c:v>
                   </c:pt>
                 </c:numCache>
               </c:numRef>
@@ -4360,13 +4432,111 @@
                 <c:formatCode>0.000</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>7.012452111392085</c:v>
+                  <c:v>7.482073562525703</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.927572232311186</c:v>
+                  <c:v>7.48506995867172</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7.92236264134766</c:v>
+                  <c:v>7.94804217325192</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="5"/>
+          <c:order val="5"/>
+          <c:tx>
+            <c:v>AFM Diagonals</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="47625">
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Human Error'!$AO$7:$AO$9</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.163079760201961</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.219580170643891</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.162238688179391</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Human Error'!$AO$7:$AO$9</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="3"/>
+                  <c:pt idx="0">
+                    <c:v>0.163079760201961</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.219580170643891</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.162238688179391</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:errBars>
+            <c:errDir val="x"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="fixedVal"/>
+            <c:noEndCap val="0"/>
+            <c:val val="1.0"/>
+          </c:errBars>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Human Error'!$AI$7:$AI$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>2942.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>490.3</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>245.2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Human Error'!$AN$7:$AN$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>5.478426600349524</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.525461676007874</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.516232898862501</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4407,6 +4577,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4441,6 +4612,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="0"/>
@@ -4458,10 +4630,10 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.435422350936142"/>
-          <c:y val="0.299048556430446"/>
-          <c:w val="0.256751541030574"/>
-          <c:h val="0.415236220472441"/>
+          <c:x val="0.422922327346915"/>
+          <c:y val="0.232381889763779"/>
+          <c:w val="0.270748478493795"/>
+          <c:h val="0.498283464566929"/>
         </c:manualLayout>
       </c:layout>
       <c:overlay val="1"/>
@@ -9868,8 +10040,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AQ21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M2" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="Q6" sqref="Q6"/>
+    <sheetView topLeftCell="T1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8:F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -10292,8 +10464,8 @@
         <v>32.744933333333336</v>
       </c>
       <c r="R8" s="45">
-        <f>B4/P8</f>
-        <v>7.0124521113920855</v>
+        <f>B4/Q8</f>
+        <v>7.4820735625257031</v>
       </c>
       <c r="S8" s="45"/>
       <c r="T8" s="42"/>
@@ -10379,12 +10551,12 @@
         <v>0.27955000149049108</v>
       </c>
       <c r="R9" s="45">
-        <f>R8*SQRT((0)^2+(P9/P8)^2)</f>
-        <v>0.13749546328856271</v>
+        <f>R8*SQRT((0)^2+(Q9/Q8)^2)</f>
+        <v>6.3875948509775266E-2</v>
       </c>
       <c r="S9" s="43">
         <f>R9/R8*100</f>
-        <v>1.9607330090025761</v>
+        <v>0.8537198675738874</v>
       </c>
       <c r="T9" s="42"/>
       <c r="U9" s="42"/>
@@ -10453,6 +10625,9 @@
       <c r="O10" s="42"/>
       <c r="P10" s="28">
         <v>67.726399999999998</v>
+      </c>
+      <c r="Q10" s="28">
+        <v>62.938800000000001</v>
       </c>
       <c r="R10" s="42"/>
       <c r="S10" s="42"/>
@@ -10502,6 +10677,9 @@
       <c r="P11" s="28">
         <v>77.476500000000001</v>
       </c>
+      <c r="Q11" s="28">
+        <v>67.726399999999998</v>
+      </c>
       <c r="R11" s="42"/>
       <c r="S11" s="42"/>
       <c r="T11" s="42"/>
@@ -10581,6 +10759,9 @@
       <c r="P12" s="28">
         <v>66.608199999999997</v>
       </c>
+      <c r="Q12" s="28">
+        <v>62.973700000000001</v>
+      </c>
       <c r="R12" s="42"/>
       <c r="S12" s="42"/>
       <c r="T12" s="42"/>
@@ -10605,11 +10786,11 @@
       </c>
       <c r="Z12" s="56">
         <f>R8</f>
-        <v>7.0124521113920855</v>
+        <v>7.4820735625257031</v>
       </c>
       <c r="AA12" s="56">
         <f>R9</f>
-        <v>0.13749546328856271</v>
+        <v>6.3875948509775266E-2</v>
       </c>
       <c r="AB12" s="42"/>
       <c r="AC12" s="42"/>
@@ -10666,6 +10847,9 @@
       <c r="P13" s="28">
         <v>71.116299999999995</v>
       </c>
+      <c r="Q13" s="28">
+        <v>68.215699999999998</v>
+      </c>
       <c r="R13" s="42"/>
       <c r="S13" s="42"/>
       <c r="T13" s="42"/>
@@ -10690,11 +10874,11 @@
       </c>
       <c r="Z13" s="56">
         <f>R14</f>
-        <v>6.9275722323111859</v>
+        <v>7.4850699586717209</v>
       </c>
       <c r="AA13" s="56">
         <f>R15</f>
-        <v>0.47872956808486555</v>
+        <v>0.33183718794899358</v>
       </c>
       <c r="AB13" s="42"/>
       <c r="AC13" s="42"/>
@@ -10755,13 +10939,13 @@
         <f>AVERAGE(P10:P13)</f>
         <v>70.731850000000009</v>
       </c>
-      <c r="Q14" s="33" t="e">
+      <c r="Q14" s="33">
         <f>AVERAGE(Q10:Q13)</f>
-        <v>#DIV/0!</v>
+        <v>65.463650000000001</v>
       </c>
       <c r="R14" s="43">
-        <f>B10/P14</f>
-        <v>6.9275722323111859</v>
+        <f>B10/Q14</f>
+        <v>7.4850699586717209</v>
       </c>
       <c r="S14" s="43"/>
       <c r="T14" s="42"/>
@@ -10786,11 +10970,11 @@
       </c>
       <c r="Z14" s="56">
         <f>R20</f>
-        <v>7.92236264134766</v>
+        <v>7.9480421732519204</v>
       </c>
       <c r="AA14" s="56">
         <f>R21</f>
-        <v>0.19460230294651493</v>
+        <v>3.0774781786817626E-2</v>
       </c>
       <c r="AB14" s="42"/>
       <c r="AC14" s="42"/>
@@ -10857,17 +11041,17 @@
         <f>STDEV(P10:P13)</f>
         <v>4.8879213185838708</v>
       </c>
-      <c r="Q15" s="34" t="e">
+      <c r="Q15" s="34">
         <f>STDEV(Q10:Q13)</f>
-        <v>#DIV/0!</v>
+        <v>2.9022138268340356</v>
       </c>
       <c r="R15" s="43">
-        <f>R14*SQRT((0)^2+(P15/P14)^2)</f>
-        <v>0.47872956808486555</v>
+        <f>R14*SQRT((0)^2+(Q15/Q14)^2)</f>
+        <v>0.33183718794899358</v>
       </c>
       <c r="S15" s="43">
         <f>R15/R14*100</f>
-        <v>6.9104955102741839</v>
+        <v>4.4333211283422722</v>
       </c>
       <c r="T15" s="42"/>
       <c r="U15" s="42"/>
@@ -10937,6 +11121,9 @@
       <c r="P16" s="7">
         <v>361.34750000000003</v>
       </c>
+      <c r="Q16" s="7">
+        <v>371.16750000000002</v>
+      </c>
       <c r="R16" s="42"/>
       <c r="S16" s="42"/>
       <c r="T16" s="42"/>
@@ -10950,7 +11137,7 @@
       <c r="Y16" s="42"/>
       <c r="Z16" s="42">
         <f>(Z12-V12)/V12*100</f>
-        <v>-5.6007310123548111</v>
+        <v>0.72115482497036332</v>
       </c>
       <c r="AA16" s="42"/>
       <c r="AB16" s="42"/>
@@ -11005,6 +11192,9 @@
       <c r="P17" s="7">
         <v>379.20519999999999</v>
       </c>
+      <c r="Q17" s="7">
+        <v>369.14060000000001</v>
+      </c>
       <c r="R17" s="42"/>
       <c r="S17" s="42"/>
       <c r="T17" s="42"/>
@@ -11018,7 +11208,7 @@
       <c r="Y17" s="42"/>
       <c r="Z17" s="42">
         <f t="shared" ref="Z17:Z18" si="1">(Z13-V13)/V13*100</f>
-        <v>-6.4941748307162888</v>
+        <v>1.0307246846150602</v>
       </c>
       <c r="AA17" s="42"/>
       <c r="AB17" s="42"/>
@@ -11092,7 +11282,7 @@
       <c r="Y18" s="42"/>
       <c r="Z18" s="42">
         <f t="shared" si="1"/>
-        <v>11.856186857171986</v>
+        <v>12.218757298481529</v>
       </c>
       <c r="AA18" s="42"/>
       <c r="AB18" s="42"/>
@@ -11203,13 +11393,13 @@
         <f>AVERAGE(P16:P19)</f>
         <v>371.35386666666665</v>
       </c>
-      <c r="Q20" s="40" t="e">
+      <c r="Q20" s="40">
         <f>AVERAGE(Q16:Q19)</f>
-        <v>#DIV/0!</v>
+        <v>370.15404999999998</v>
       </c>
       <c r="R20" s="45">
-        <f>B16/P20</f>
-        <v>7.92236264134766</v>
+        <f>B16/Q20</f>
+        <v>7.9480421732519204</v>
       </c>
       <c r="S20" s="45"/>
       <c r="T20" s="42"/>
@@ -11285,17 +11475,17 @@
         <f>STDEV(P16:P19)</f>
         <v>9.1218138998410279</v>
       </c>
-      <c r="Q21" s="19" t="e">
+      <c r="Q21" s="19">
         <f>STDEV(Q16:Q19)</f>
-        <v>#DIV/0!</v>
+        <v>1.4332347347870218</v>
       </c>
       <c r="R21" s="45">
-        <f>R20*SQRT((0)^2+(P21/P20)^2)</f>
-        <v>0.19460230294651493</v>
+        <f>R20*SQRT((0)^2+(Q21/Q20)^2)</f>
+        <v>3.0774781786817626E-2</v>
       </c>
       <c r="S21" s="43">
         <f>R21/R20*100</f>
-        <v>2.4563670177235339</v>
+        <v>0.3871995280848668</v>
       </c>
       <c r="T21" s="42"/>
       <c r="U21" s="42"/>
@@ -11338,8 +11528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:AO24"/>
   <sheetViews>
-    <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="AP20" sqref="AP20"/>
+    <sheetView tabSelected="1" topLeftCell="AG7" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="AA7" sqref="AA7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -11355,6 +11545,7 @@
     <col min="37" max="37" width="11.1640625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="6.5" bestFit="1" customWidth="1"/>
     <col min="39" max="39" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:41">
@@ -11482,8 +11673,12 @@
       <c r="AM6" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="AN6" s="2"/>
-      <c r="AO6" s="2"/>
+      <c r="AN6" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="AO6" s="2" t="s">
+        <v>96</v>
+      </c>
     </row>
     <row r="7" spans="2:41">
       <c r="B7" s="23">
@@ -11610,6 +11805,14 @@
         <f>X12</f>
         <v>7.1116871388159725E-2</v>
       </c>
+      <c r="AN7" s="3">
+        <f>Diagonals!J22</f>
+        <v>5.4784266003495246</v>
+      </c>
+      <c r="AO7" s="3">
+        <f>Diagonals!J23</f>
+        <v>0.16307976020196088</v>
+      </c>
     </row>
     <row r="8" spans="2:41">
       <c r="B8" s="23">
@@ -11736,6 +11939,14 @@
         <f>X18</f>
         <v>0.12771083964972155</v>
       </c>
+      <c r="AN8" s="3">
+        <f>Diagonals!J16</f>
+        <v>5.5254616760078736</v>
+      </c>
+      <c r="AO8" s="3">
+        <f>Diagonals!J17</f>
+        <v>0.21958017064389102</v>
+      </c>
     </row>
     <row r="9" spans="2:41">
       <c r="B9" s="23">
@@ -11861,6 +12072,14 @@
       <c r="AM9" s="3">
         <f>X24</f>
         <v>0.109401357751937</v>
+      </c>
+      <c r="AN9" s="3">
+        <f>Diagonals!J10</f>
+        <v>5.5162328988625013</v>
+      </c>
+      <c r="AO9" s="3">
+        <f>Diagonals!J11</f>
+        <v>0.16223868817939138</v>
       </c>
     </row>
     <row r="10" spans="2:41">
@@ -12869,4 +13088,298 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B4:J23"/>
+  <sheetViews>
+    <sheetView topLeftCell="C3" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="9" max="9" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:10">
+      <c r="B4" t="s">
+        <v>89</v>
+      </c>
+      <c r="G4" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="5" spans="2:10">
+      <c r="B5" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+      <c r="H5" t="s">
+        <v>1</v>
+      </c>
+      <c r="I5" t="s">
+        <v>88</v>
+      </c>
+      <c r="J5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="6" spans="2:10">
+      <c r="B6" t="s">
+        <v>91</v>
+      </c>
+      <c r="C6" s="50">
+        <v>550.92100000000005</v>
+      </c>
+      <c r="G6">
+        <v>245.2</v>
+      </c>
+      <c r="H6">
+        <v>1</v>
+      </c>
+      <c r="I6">
+        <v>45.0364</v>
+      </c>
+    </row>
+    <row r="7" spans="2:10">
+      <c r="B7" t="s">
+        <v>92</v>
+      </c>
+      <c r="C7" s="50">
+        <v>551.08040000000005</v>
+      </c>
+      <c r="G7">
+        <v>245.2</v>
+      </c>
+      <c r="H7">
+        <v>2</v>
+      </c>
+      <c r="I7">
+        <v>42.942700000000002</v>
+      </c>
+    </row>
+    <row r="8" spans="2:10">
+      <c r="B8" t="s">
+        <v>93</v>
+      </c>
+      <c r="C8" s="50">
+        <v>550.83600000000001</v>
+      </c>
+      <c r="G8">
+        <v>245.2</v>
+      </c>
+      <c r="H8">
+        <v>3</v>
+      </c>
+      <c r="I8">
+        <v>45.9328</v>
+      </c>
+    </row>
+    <row r="9" spans="2:10">
+      <c r="B9" t="s">
+        <v>94</v>
+      </c>
+      <c r="C9" s="50">
+        <v>550.93010000000004</v>
+      </c>
+      <c r="G9">
+        <v>245.2</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>43.890599999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="2:10">
+      <c r="B10" t="s">
+        <v>34</v>
+      </c>
+      <c r="C10" s="3">
+        <f>AVERAGE(C6:C9)</f>
+        <v>550.94187499999998</v>
+      </c>
+      <c r="H10" t="s">
+        <v>34</v>
+      </c>
+      <c r="I10" s="3">
+        <f>AVERAGE(I6:I9)</f>
+        <v>44.450625000000002</v>
+      </c>
+      <c r="J10" s="43">
+        <f>G6/I10</f>
+        <v>5.5162328988625013</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10">
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11" s="3">
+        <f>STDEV(C6:C9)</f>
+        <v>0.10160890298920557</v>
+      </c>
+      <c r="H11" t="s">
+        <v>95</v>
+      </c>
+      <c r="I11" s="3">
+        <f>STDEV(I6:I9)</f>
+        <v>1.3073434753346185</v>
+      </c>
+      <c r="J11" s="43">
+        <f>J10*SQRT((0)^2+(I11/I10)^2)</f>
+        <v>0.16223868817939138</v>
+      </c>
+    </row>
+    <row r="12" spans="2:10">
+      <c r="G12">
+        <v>490.3</v>
+      </c>
+      <c r="H12">
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <v>85.480800000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="2:10">
+      <c r="G13">
+        <v>490.3</v>
+      </c>
+      <c r="H13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="2:10">
+      <c r="G14">
+        <v>490.3</v>
+      </c>
+      <c r="H14">
+        <v>3</v>
+      </c>
+      <c r="I14">
+        <v>92.481499999999997</v>
+      </c>
+    </row>
+    <row r="15" spans="2:10">
+      <c r="G15">
+        <v>490.3</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>88.241699999999994</v>
+      </c>
+    </row>
+    <row r="16" spans="2:10">
+      <c r="H16" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="3">
+        <f>AVERAGE(I12:I15)</f>
+        <v>88.734666666666669</v>
+      </c>
+      <c r="J16" s="43">
+        <f>G12/I16</f>
+        <v>5.5254616760078736</v>
+      </c>
+    </row>
+    <row r="17" spans="7:10">
+      <c r="H17" t="s">
+        <v>95</v>
+      </c>
+      <c r="I17" s="3">
+        <f>STDEV(I12:I15)</f>
+        <v>3.5262887322698515</v>
+      </c>
+      <c r="J17" s="43">
+        <f>J16*SQRT((0)^2+(I17/I16)^2)</f>
+        <v>0.21958017064389102</v>
+      </c>
+    </row>
+    <row r="18" spans="7:10">
+      <c r="G18">
+        <v>2942</v>
+      </c>
+      <c r="H18">
+        <v>1</v>
+      </c>
+      <c r="I18">
+        <v>543.50530000000003</v>
+      </c>
+    </row>
+    <row r="19" spans="7:10">
+      <c r="G19">
+        <v>2942</v>
+      </c>
+      <c r="H19">
+        <v>2</v>
+      </c>
+      <c r="I19">
+        <v>514.1105</v>
+      </c>
+    </row>
+    <row r="20" spans="7:10">
+      <c r="G20">
+        <v>2942</v>
+      </c>
+      <c r="H20">
+        <v>3</v>
+      </c>
+      <c r="I20">
+        <v>539.51610000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="7:10">
+      <c r="G21">
+        <v>2942</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21" s="50">
+        <v>550.93010000000004</v>
+      </c>
+    </row>
+    <row r="22" spans="7:10">
+      <c r="H22" t="s">
+        <v>34</v>
+      </c>
+      <c r="I22" s="3">
+        <f>AVERAGE(I18:I21)</f>
+        <v>537.01549999999997</v>
+      </c>
+      <c r="J22" s="43">
+        <f>G18/I22</f>
+        <v>5.4784266003495246</v>
+      </c>
+    </row>
+    <row r="23" spans="7:10">
+      <c r="H23" t="s">
+        <v>95</v>
+      </c>
+      <c r="I23" s="3">
+        <f>STDEV(I18:I21)</f>
+        <v>15.985677157589139</v>
+      </c>
+      <c r="J23" s="43">
+        <f>J22*SQRT((0)^2+(I23/I22)^2)</f>
+        <v>0.16307976020196088</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>